<commit_message>
Implement fix bug import student to group module
</commit_message>
<xml_diff>
--- a/src/assets/files/DanhSachSinhVien.xlsx
+++ b/src/assets/files/DanhSachSinhVien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34BA0B2-16BA-4658-A179-F9743024CACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4B23DF-1F65-4F37-A263-E977C9C51873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19905" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Danh sách sinh viên" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>MSSV</t>
   </si>
@@ -34,28 +34,43 @@
     <t>Số điện thoại</t>
   </si>
   <si>
-    <t>Ngày tham gia</t>
+    <t>Giới tính</t>
+  </si>
+  <si>
+    <t>Ngày sinh</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
   </si>
   <si>
     <t>Nguyễn Đình Hùng</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Phạm Thanh Long</t>
   </si>
   <si>
     <t>Bùi Xuân Hoàng</t>
   </si>
   <si>
-    <t>dangdang22@gmail.com</t>
-  </si>
-  <si>
-    <t>dangdang23@gmail.com</t>
-  </si>
-  <si>
-    <t>dangdang33@gmail.com</t>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>Hưng Yên</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>nguyendinhhungzz@gmail.com</t>
+  </si>
+  <si>
+    <t>phamthanhlongê@gmail.com</t>
+  </si>
+  <si>
+    <t>buixuanhoangyy@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -106,9 +121,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -425,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -437,10 +453,12 @@
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,63 +474,87 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2">
-        <v>10121917</v>
+        <v>12520011</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>2385785342</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>37535</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>12520012</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>1385785342</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
+        <v>37562</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>12520013</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
-        <v>61922002333</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>10121919</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>76922002223</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>10121918</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>5385785342</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
-        <v>89922002115</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
+      <c r="F4" s="2">
+        <v>37351</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{9BB833ED-9AE6-46B6-BB4E-8EEF9E459356}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{DE90CE42-0880-41AA-A5BD-0646BF0A7A11}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{ADC299AF-93E5-453D-8B36-FC8D4C4292D7}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{DC96DB58-C435-4D6C-B1E2-6DCEF298BA20}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{281F8253-1A7D-4477-AA91-CBE6B29B4E0C}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{0AE0CADD-07DE-4D91-ACAC-F875F5B4ADAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>